<commit_message>
after showing elowyn the calibration curve
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/manual_calibrations_combined.xlsx
+++ b/Hydrophones/Calibration/manual_calibrations_combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001E45AA-2BD4-4237-8E43-1CEA21191FAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B726B842-1E09-4275-A6ED-809960B0F1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H1_impact_pipe" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>Particle #</t>
   </si>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -177,7 +177,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,10 +500,10 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,6 +621,12 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>3.0499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.6E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,9 +963,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>Floods</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:noFill/>
@@ -985,17 +991,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$B$38:$B$40</c:f>
+              <c:f>H1_impact_pipe!$B$38:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -1003,10 +1015,22 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$F$38:$F$40</c:f>
+              <c:f>H1_impact_pipe!$F$38:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>4.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0099999999999999E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1153,6 +1177,7 @@
       <c:valAx>
         <c:axId val="299627312"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1476,10 +1501,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$B$2:$B$40</c:f>
+              <c:f>H1_impact_pipe!$B$2:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>128</c:v>
                 </c:pt>
@@ -1592,9 +1617,15 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="37">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="38">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="39">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -1602,10 +1633,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$E$2:$E$40</c:f>
+              <c:f>H1_impact_pipe!$E$2:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>7.0800000000000002E-2</c:v>
                 </c:pt>
@@ -1713,6 +1744,18 @@
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>2.93E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.7999999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.9599999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,9 +2086,6 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
-          <c:tx>
-            <c:v>Floods</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -2074,17 +2114,23 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$B$38:$B$40</c:f>
+              <c:f>H1_impact_pipe!$B$38:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -2092,10 +2138,22 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>H1_impact_pipe!$F$38:$F$40</c:f>
+              <c:f>H1_impact_pipe!$F$38:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>4.87E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0099999999999999E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2242,6 +2300,7 @@
       <c:valAx>
         <c:axId val="299627312"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4682,7 +4741,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4762,7 +4821,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-AR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4888,7 +4947,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1128790880"/>
@@ -4950,7 +5009,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1128790400"/>
@@ -4998,7 +5057,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7941,16 +8000,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>169545</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>560070</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>436245</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8241,10 +8300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I40"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9050,31 +9109,70 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="1">
+      <c r="A38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="5">
         <v>90</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45</v>
-      </c>
-      <c r="F39" s="1"/>
+      <c r="A39" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="5">
+        <v>90</v>
+      </c>
+      <c r="E39" s="5">
+        <v>4.87E-2</v>
+      </c>
+      <c r="F39" s="5">
+        <v>4.87E-2</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="5">
+        <v>45</v>
+      </c>
+      <c r="E40" s="5">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="F40" s="5">
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="5">
+        <v>64</v>
+      </c>
+      <c r="E41" s="5">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F41" s="5">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B42" s="5">
         <v>90</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="E42" s="5">
+        <v>4.9599999999999998E-2</v>
+      </c>
+      <c r="F42" s="5">
+        <v>5.0099999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9087,7 +9185,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9924,8 +10022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE41D157-6BBB-47F7-AC96-7DF3592F224F}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9940,18 +10038,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="5"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -10078,18 +10176,18 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">

</xml_diff>